<commit_message>
update results with fixed bug
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/results/improvements/local_optimum.xlsx
+++ b/dmsan/bwaise/results/improvements/local_optimum.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/bwaise/results/improvements/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_821427AF91E6E8BF891C873C42AA7393D1B2142F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{069D6349-D55A-3747-AE4B-6B5568023530}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="15000" yWindow="4000" windowWidth="20980" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>T1</t>
   </si>
@@ -26,6 +32,9 @@
   </si>
   <si>
     <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
   </si>
   <si>
     <t>T6</t>
@@ -94,8 +103,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,13 +120,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -147,9 +175,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -158,6 +194,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -204,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,9 +280,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,6 +332,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,14 +525,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -465,478 +547,429 @@
       <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.052</v>
+        <v>0.08</v>
       </c>
       <c r="C2">
-        <v>0.166</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="D2">
-        <v>0.398</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="E2">
-        <v>0.77</v>
-      </c>
-      <c r="F2">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.049</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C3">
-        <v>0.157</v>
+        <v>0.45</v>
       </c>
       <c r="D3">
-        <v>0.392</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="E3">
-        <v>0.764</v>
-      </c>
-      <c r="F3">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0.049</v>
-      </c>
-      <c r="C4">
-        <v>0.157</v>
-      </c>
-      <c r="D4">
-        <v>0.397</v>
-      </c>
-      <c r="E4">
-        <v>0.767</v>
-      </c>
-      <c r="F4">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="B4" s="3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.05</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C5">
-        <v>0.158</v>
+        <v>0.45</v>
       </c>
       <c r="D5">
-        <v>0.397</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="E5">
-        <v>0.769</v>
-      </c>
-      <c r="F5">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.051</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="C6">
-        <v>0.166</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="D6">
-        <v>0.398</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="E6">
-        <v>0.77</v>
-      </c>
-      <c r="F6">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.88600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.049</v>
+        <v>0.08</v>
       </c>
       <c r="C7">
-        <v>0.157</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="D7">
-        <v>0.397</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="E7">
-        <v>0.767</v>
-      </c>
-      <c r="F7">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0.067</v>
-      </c>
-      <c r="C8">
-        <v>0.176</v>
-      </c>
-      <c r="D8">
-        <v>0.411</v>
-      </c>
-      <c r="E8">
-        <v>0.78</v>
-      </c>
-      <c r="F8">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="B8" s="3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.073</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="C9">
-        <v>0.181</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="D9">
-        <v>0.419</v>
+        <v>0.66</v>
       </c>
       <c r="E9">
-        <v>0.786</v>
-      </c>
-      <c r="F9">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.11</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="C10">
-        <v>0.227</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="D10">
-        <v>0.579</v>
+        <v>0.66400000000000003</v>
       </c>
       <c r="E10">
-        <v>0.988</v>
-      </c>
-      <c r="F10">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>0.88600000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.049</v>
+        <v>0.156</v>
       </c>
       <c r="C11">
-        <v>0.159</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="D11">
-        <v>0.407</v>
+        <v>0.78100000000000003</v>
       </c>
       <c r="E11">
-        <v>0.8</v>
-      </c>
-      <c r="F11">
-        <v>0.994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.049</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C12">
-        <v>0.159</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="D12">
-        <v>0.405</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="E12">
-        <v>0.794</v>
-      </c>
-      <c r="F12">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>0.89600000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.049</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C13">
-        <v>0.157</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="D13">
-        <v>0.398</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="E13">
-        <v>0.769</v>
-      </c>
-      <c r="F13">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>0.89400000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.132</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C14">
-        <v>0.249</v>
+        <v>0.45</v>
       </c>
       <c r="D14">
-        <v>0.61</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="E14">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.049</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="C15">
-        <v>0.158</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="D15">
-        <v>0.404</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="E15">
-        <v>0.785</v>
-      </c>
-      <c r="F15">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.049</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C16">
-        <v>0.157</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="D16">
-        <v>0.397</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="E16">
-        <v>0.767</v>
-      </c>
-      <c r="F16">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>0.049</v>
-      </c>
-      <c r="C17">
-        <v>0.159</v>
-      </c>
-      <c r="D17">
-        <v>0.403</v>
-      </c>
-      <c r="E17">
-        <v>0.77</v>
-      </c>
-      <c r="F17">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="B17" s="3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.135</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C18">
-        <v>0.397</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1" t="s">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="E18">
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="C19">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.049</v>
-      </c>
-      <c r="C20">
-        <v>0.157</v>
-      </c>
-      <c r="D20">
-        <v>0.398</v>
-      </c>
-      <c r="E20">
-        <v>0.772</v>
-      </c>
-      <c r="F20">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.109</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C21">
-        <v>0.24</v>
+        <v>0.45</v>
       </c>
       <c r="D21">
-        <v>0.767</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E21">
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.049</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="C22">
-        <v>0.157</v>
+        <v>0.626</v>
       </c>
       <c r="D22">
-        <v>0.397</v>
-      </c>
-      <c r="E22">
-        <v>0.767</v>
-      </c>
-      <c r="F22">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>0.052</v>
-      </c>
-      <c r="C23">
-        <v>0.168</v>
-      </c>
-      <c r="D23">
-        <v>0.426</v>
-      </c>
-      <c r="E23">
-        <v>0.848</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="B23" s="3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.055</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="C24">
-        <v>0.181</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="D24">
-        <v>0.516</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="E24">
-        <v>0.837</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>0.89800000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.048</v>
+        <v>0.08</v>
       </c>
       <c r="C25">
-        <v>0.148</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="D25">
-        <v>0.351</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="E25">
-        <v>0.78</v>
-      </c>
-      <c r="F25">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>0.89600000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>0.053</v>
-      </c>
-      <c r="C26">
-        <v>0.17</v>
-      </c>
-      <c r="D26">
-        <v>0.446</v>
+      <c r="B26" s="4">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.61599999999999999</v>
       </c>
       <c r="E26">
-        <v>0.8149999999999999</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
+        <v>0.88700000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="C27">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="D27">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="E27">
+        <v>0.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>